<commit_message>
penambahan data judul inggris
</commit_message>
<xml_diff>
--- a/S1 Keperawatan/RPL/RPL 3/Transkip Nilai RPL3.xlsx
+++ b/S1 Keperawatan/RPL/RPL 3/Transkip Nilai RPL3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\S1 Keperawatan\RPL\RPL 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{308126DB-8070-4EC3-9D42-1866750C43D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3092F6C-8A8B-4C82-B8C7-77894CA22E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6728395-340D-414D-8D40-C463D1B813FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="317">
   <si>
     <t>NO</t>
   </si>
@@ -732,9 +732,6 @@
     <t>7 November 2025</t>
   </si>
   <si>
-    <t>wirdani</t>
-  </si>
-  <si>
     <t xml:space="preserve">Namu Sira Sira </t>
   </si>
   <si>
@@ -847,6 +844,147 @@
   </si>
   <si>
     <t>Kusmarsari</t>
+  </si>
+  <si>
+    <t>Judul Inggris</t>
+  </si>
+  <si>
+    <t>Factors Influencing Salt Intake Compliance Among Diabetes Mellitus Patients in the Sedanao Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>Factors Affecting the Quality of Health Services on Outpatient Satisfaction at the Sedanao Primary Health Care Center Technical Implementation Unit (UPTD)</t>
+  </si>
+  <si>
+    <t>The Effect of Broiler Egg Supplementary Feeding on Body Weight Levels of Stunted Children in the Serasan Primary Health Care Center Working Area, Natuna Regency</t>
+  </si>
+  <si>
+    <t>The Relationship between Preventive Behavior and the Incidence of HIV/AIDS Among Female Commercial Sex Workers in Ranai</t>
+  </si>
+  <si>
+    <t>The Correlation between Self-Management and Blood Pressure in Hypertensive Patients in the Ranai Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>The Effect of Diet Management on Hypertension Diet Compliance and Achievement in Tanjung Village, Pulau Laut Primary Health Care Center UPTD Working Area, Natuna Regency in 2025</t>
+  </si>
+  <si>
+    <t>The Effect of Motivational Interviewing (MI) on Improving Compliance in Preoperative Patients Scheduled for Effective Local Anesthesia at Raja Ahmad Tabib Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Effect of Cupping Therapy on Cholesterol Levels in Hypercholesterolemia Patients in Bandarsyah Village</t>
+  </si>
+  <si>
+    <t>Factors Influencing Patient Satisfaction with the Quality of Services at Batu Jaya Primary Health Care Center, Natuna Regency</t>
+  </si>
+  <si>
+    <t>The Relationship between Response Time and Anxiety Level in Emergency Department Patients at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Correlation between Work Motivation and Incentive Funds (Bok) with Nurse Performance at the Sedanao Primary Health Care Center UPTD</t>
+  </si>
+  <si>
+    <t>Risk Factors Associated with the Occurrence of Malaria Relapse in Kampung Bugis Village</t>
+  </si>
+  <si>
+    <t>The Relationship between Family Support, Self-Efficacy, and Medication Adherence in Pulmonary Tuberculosis Patients at the Ranai Primary Health Care Center UPTD</t>
+  </si>
+  <si>
+    <t>The Correlation between Dietary Patterns, Physical Activity, and the Incidence of Coronary Heart Disease at the Cardiac Clinic of Raja Ahmad Tabib Regional General Hospital, Tanjungpinang City, Riau Islands Province</t>
+  </si>
+  <si>
+    <t>The Relationship between Length of Infant Hospitalization, Family Support, and Parental Anxiety Levels in the NICU Room of Natuna Regional General Hospital in 2025</t>
+  </si>
+  <si>
+    <t>The Effect of Work Motivation Program on Employee Performance at the Ranai Primary Health Care Center UPTD</t>
+  </si>
+  <si>
+    <t>The Relationship between Knowledge Level about Hypertension and Hypertension Complication Prevention Behavior at the BKK Class I Tanjungpinang Port Working Area</t>
+  </si>
+  <si>
+    <t>Factors Related to Drug Abuse Among Inmates at the Class I State Detention Center, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>The Effect of the Cerdik Program on Blood Pressure in Hypertensive Patients at the Midai Primary Health Care Center</t>
+  </si>
+  <si>
+    <t>A Phenomenological Study: Phenomena and Family Experiences in Caring for Patients with Schizophrenia in the Natuna Coastal Community Area</t>
+  </si>
+  <si>
+    <t>The Correlation between Socio-Cultural Factors and Efforts to Prevent the Transmission of Pulmonary Tuberculosis in the Serasan Timur Primary Health Care Center, Natuna Regency</t>
+  </si>
+  <si>
+    <t>The Relationship between Knowledge and Healthy Lifestyle Behavior with the Incidence of Gastritis in the Outpatient Department of Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>Factors Related to the Incidence of Chronic Energy Deficiency (CED) in Pregnant Women in the Pulau Serasan Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>The Effect of Intradialytic Exercise on Fatigue in Chronic Kidney Disease Patients Undergoing Hemodialysis Therapy at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Effect of Education using the Demonstration Method on the Level of Early Mobilization Independence in Post-Operative Patients at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Effect of Early Mobilization on the Inflammatory Phase Wound Healing Time in Post-Operative Patients in the Surgical Inpatient Room of Tanjungpinang Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Effect of Health Education through Video on Anxiety in Pre-Operative Sectio Caesarea Mothers at Natuna District General Hospital</t>
+  </si>
+  <si>
+    <t>The Relationship between Duration of Illness and Quality of Life in Type II Diabetes Mellitus Patients in the Outpatient Department of Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Relationship between the Role of Elderly Cadres and Family Support with Elderly Visits to the Elderly Posyandu in the Sedanau Primary Health Care Center UPTD Working Area in 2025</t>
+  </si>
+  <si>
+    <t>The Correlation between Consumption of Risky Foods and the Incidence of Tonsillitis in School-Age Children at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Effect of Blanket Warmer Use on Postoperative Hypothermia in the Recovery Room of Natuna District General Hospital</t>
+  </si>
+  <si>
+    <t>Factors Associated with the Incidence of Acute Respiratory Infection (ARI) in Toddlers in the Bunguran Tengah Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>The Effect of Preoperative Skin Preparation using 0.5% Chlorhexidine on the Inflammatory Phase Wound Healing Process in Post-Laparotomy Patients at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Effect of Healthy Lifestyle Education on Adolescents' Knowledge Level of Early Hypertension Prevention in Pulau Laut Sub-district</t>
+  </si>
+  <si>
+    <t>The Relationship between Family Support and Medication Adherence in Pulmonary Tuberculosis Patients at Melayu Primary Health Care Center, Tanjungpinang City</t>
+  </si>
+  <si>
+    <t>The Correlation between Health Literacy, Self-Efficacy, and Adherence to Taking Blood Supplement Tablets Among Female Adolescents at Bunguran Barat High School, Sedanao Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>The Relationship between Anxiety and Fatigue in Stage V Chronic Kidney Disease (CKD) Patients Undergoing Hemodialysis at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Relationship between Family Role and Medication Adherence in Elderly Hypertensive Patients in Ranai Kota Village</t>
+  </si>
+  <si>
+    <t>The Correlation between Lifestyle and the Risk of Hypertension in Adolescents in the Ranai Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>Factors Related to Toddler Visits to Posyandu (Integrated Health Post) in the Ranai Primary Health Care Center Working Area</t>
+  </si>
+  <si>
+    <t>Factors Influencing Self-Management in Stroke Patients at Bintan District Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Relationship between Parental Presence and Child Anxiety During Intravenous Line Medication Administration in the Pediatric Inpatient Room of Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Correlation between Medication Adherence and Relapse in Schizophrenia Patients in Natuna Regency in 2025</t>
+  </si>
+  <si>
+    <t>The Relationship between Family Support and Quality of Life in Stage V Chronic Kidney Failure Patients Undergoing Hemodialysis at Natuna Regional General Hospital</t>
+  </si>
+  <si>
+    <t>The Correlation between Mothers' Knowledge and Adherence to Completing Advanced Immunizations in Toddlers in the Ranai Primary Health Care Center Working Area, Bunguran Timur Sub-district, Natuna Regency</t>
+  </si>
+  <si>
+    <t>The Relationship between Anxiety and Hypertension Compliance in Elderly Women in the Sedanau Primary Health Care Center UPTD Working Area</t>
   </si>
 </sst>
 </file>
@@ -1067,29 +1205,29 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1406,20 +1544,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7BDEEA-51B9-444E-8343-089DD6E8FAC7}">
-  <dimension ref="A1:DX53"/>
+  <dimension ref="A1:DY50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="DX24" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="CI3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B2"/>
+      <selection pane="bottomRight" activeCell="DA21" sqref="DA21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="41" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" style="35" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" style="4" customWidth="1"/>
     <col min="5" max="6" width="20.28515625" style="9" customWidth="1"/>
     <col min="7" max="7" width="20.28515625" style="4" customWidth="1"/>
@@ -1443,20 +1581,21 @@
     <col min="126" max="126" width="18.28515625" style="4" customWidth="1"/>
     <col min="127" max="127" width="18.140625" style="4" customWidth="1"/>
     <col min="128" max="128" width="186.85546875" style="27" bestFit="1" customWidth="1"/>
-    <col min="129" max="16384" width="9.140625" style="4"/>
+    <col min="129" max="129" width="198.7109375" style="27" bestFit="1" customWidth="1"/>
+    <col min="130" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" x14ac:dyDescent="0.25">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:129" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="34" t="s">
+      <c r="C1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>66</v>
       </c>
       <c r="E1" s="38" t="s">
@@ -1465,201 +1604,204 @@
       <c r="F1" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="G1" s="34" t="s">
+      <c r="G1" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
-      <c r="M1" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
-      <c r="P1" s="33"/>
-      <c r="Q1" s="33"/>
-      <c r="R1" s="33" t="s">
+      <c r="H1" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37" t="s">
+        <v>4</v>
+      </c>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="S1" s="33"/>
-      <c r="T1" s="33"/>
-      <c r="U1" s="33"/>
-      <c r="V1" s="33"/>
-      <c r="W1" s="33" t="s">
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="33"/>
-      <c r="Y1" s="33"/>
-      <c r="Z1" s="33"/>
-      <c r="AA1" s="33"/>
-      <c r="AB1" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="AC1" s="33"/>
-      <c r="AD1" s="33"/>
-      <c r="AE1" s="33"/>
-      <c r="AF1" s="33"/>
-      <c r="AG1" s="33" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33" t="s">
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="AR1" s="33"/>
-      <c r="AS1" s="33"/>
-      <c r="AT1" s="33"/>
-      <c r="AU1" s="33"/>
-      <c r="AV1" s="33" t="s">
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="AW1" s="33"/>
-      <c r="AX1" s="33"/>
-      <c r="AY1" s="33"/>
-      <c r="AZ1" s="33"/>
-      <c r="BA1" s="33" t="s">
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="BB1" s="33"/>
-      <c r="BC1" s="33"/>
-      <c r="BD1" s="33"/>
-      <c r="BE1" s="33"/>
-      <c r="BF1" s="33" t="s">
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="37"/>
+      <c r="BF1" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="BG1" s="33"/>
-      <c r="BH1" s="33"/>
-      <c r="BI1" s="33"/>
-      <c r="BJ1" s="33"/>
-      <c r="BK1" s="33" t="s">
+      <c r="BG1" s="37"/>
+      <c r="BH1" s="37"/>
+      <c r="BI1" s="37"/>
+      <c r="BJ1" s="37"/>
+      <c r="BK1" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="BL1" s="33"/>
-      <c r="BM1" s="33"/>
-      <c r="BN1" s="33"/>
-      <c r="BO1" s="33"/>
-      <c r="BP1" s="33" t="s">
+      <c r="BL1" s="37"/>
+      <c r="BM1" s="37"/>
+      <c r="BN1" s="37"/>
+      <c r="BO1" s="37"/>
+      <c r="BP1" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="BQ1" s="33"/>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="33" t="s">
+      <c r="BQ1" s="37"/>
+      <c r="BR1" s="37"/>
+      <c r="BS1" s="37"/>
+      <c r="BT1" s="37"/>
+      <c r="BU1" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="BV1" s="33"/>
-      <c r="BW1" s="33"/>
-      <c r="BX1" s="33"/>
-      <c r="BY1" s="33"/>
-      <c r="BZ1" s="33" t="s">
+      <c r="BV1" s="37"/>
+      <c r="BW1" s="37"/>
+      <c r="BX1" s="37"/>
+      <c r="BY1" s="37"/>
+      <c r="BZ1" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="CA1" s="33"/>
-      <c r="CB1" s="33"/>
-      <c r="CC1" s="33"/>
-      <c r="CD1" s="33"/>
-      <c r="CE1" s="33" t="s">
+      <c r="CA1" s="37"/>
+      <c r="CB1" s="37"/>
+      <c r="CC1" s="37"/>
+      <c r="CD1" s="37"/>
+      <c r="CE1" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="CF1" s="33"/>
-      <c r="CG1" s="33"/>
-      <c r="CH1" s="33"/>
-      <c r="CI1" s="33"/>
-      <c r="CJ1" s="33" t="s">
+      <c r="CF1" s="37"/>
+      <c r="CG1" s="37"/>
+      <c r="CH1" s="37"/>
+      <c r="CI1" s="37"/>
+      <c r="CJ1" s="37" t="s">
         <v>76</v>
       </c>
-      <c r="CK1" s="33"/>
-      <c r="CL1" s="33"/>
-      <c r="CM1" s="33"/>
-      <c r="CN1" s="33"/>
-      <c r="CO1" s="33" t="s">
+      <c r="CK1" s="37"/>
+      <c r="CL1" s="37"/>
+      <c r="CM1" s="37"/>
+      <c r="CN1" s="37"/>
+      <c r="CO1" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="CP1" s="33"/>
-      <c r="CQ1" s="33"/>
-      <c r="CR1" s="33"/>
-      <c r="CS1" s="33"/>
-      <c r="CT1" s="33" t="s">
+      <c r="CP1" s="37"/>
+      <c r="CQ1" s="37"/>
+      <c r="CR1" s="37"/>
+      <c r="CS1" s="37"/>
+      <c r="CT1" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="CU1" s="33"/>
-      <c r="CV1" s="33"/>
-      <c r="CW1" s="33"/>
-      <c r="CX1" s="33"/>
-      <c r="CY1" s="33" t="s">
+      <c r="CU1" s="37"/>
+      <c r="CV1" s="37"/>
+      <c r="CW1" s="37"/>
+      <c r="CX1" s="37"/>
+      <c r="CY1" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="CZ1" s="33"/>
-      <c r="DA1" s="33"/>
-      <c r="DB1" s="33"/>
-      <c r="DC1" s="33"/>
-      <c r="DD1" s="33" t="s">
+      <c r="CZ1" s="37"/>
+      <c r="DA1" s="37"/>
+      <c r="DB1" s="37"/>
+      <c r="DC1" s="37"/>
+      <c r="DD1" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="DE1" s="33"/>
-      <c r="DF1" s="33"/>
-      <c r="DG1" s="33"/>
-      <c r="DH1" s="33"/>
-      <c r="DI1" s="33" t="s">
+      <c r="DE1" s="37"/>
+      <c r="DF1" s="37"/>
+      <c r="DG1" s="37"/>
+      <c r="DH1" s="37"/>
+      <c r="DI1" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="DJ1" s="33"/>
-      <c r="DK1" s="33"/>
-      <c r="DL1" s="33"/>
-      <c r="DM1" s="33"/>
-      <c r="DN1" s="37" t="s">
+      <c r="DJ1" s="37"/>
+      <c r="DK1" s="37"/>
+      <c r="DL1" s="37"/>
+      <c r="DM1" s="37"/>
+      <c r="DN1" s="39" t="s">
         <v>167</v>
       </c>
-      <c r="DO1" s="37"/>
-      <c r="DP1" s="34" t="s">
+      <c r="DO1" s="39"/>
+      <c r="DP1" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="DQ1" s="34"/>
-      <c r="DR1" s="34" t="s">
+      <c r="DQ1" s="36"/>
+      <c r="DR1" s="36" t="s">
         <v>83</v>
       </c>
-      <c r="DS1" s="34" t="s">
+      <c r="DS1" s="36" t="s">
         <v>84</v>
       </c>
-      <c r="DT1" s="34" t="s">
+      <c r="DT1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="DU1" s="35" t="s">
+      <c r="DU1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="DV1" s="36" t="s">
+      <c r="DV1" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="DW1" s="36" t="s">
+      <c r="DW1" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="DX1" s="35" t="s">
+      <c r="DX1" s="40" t="s">
         <v>144</v>
       </c>
+      <c r="DY1" s="41" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="2" spans="1:128" x14ac:dyDescent="0.25">
-      <c r="A2" s="34"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
+    <row r="2" spans="1:129" x14ac:dyDescent="0.25">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="38"/>
       <c r="F2" s="38"/>
-      <c r="G2" s="34"/>
+      <c r="G2" s="36"/>
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
@@ -2002,15 +2144,16 @@
       <c r="DQ2" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="DR2" s="34"/>
-      <c r="DS2" s="34"/>
-      <c r="DT2" s="34"/>
-      <c r="DU2" s="35"/>
-      <c r="DV2" s="36"/>
-      <c r="DW2" s="36"/>
-      <c r="DX2" s="35"/>
+      <c r="DR2" s="36"/>
+      <c r="DS2" s="36"/>
+      <c r="DT2" s="36"/>
+      <c r="DU2" s="40"/>
+      <c r="DV2" s="41"/>
+      <c r="DW2" s="41"/>
+      <c r="DX2" s="40"/>
+      <c r="DY2" s="41"/>
     </row>
-    <row r="3" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A3" s="29">
         <v>1</v>
       </c>
@@ -2468,10 +2611,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX3" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
+      </c>
+      <c r="DY3" s="25" t="s">
+        <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A4" s="29">
         <v>2</v>
       </c>
@@ -2929,10 +3075,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX4" s="25" t="s">
-        <v>260</v>
+        <v>259</v>
+      </c>
+      <c r="DY4" s="25" t="s">
+        <v>272</v>
       </c>
     </row>
-    <row r="5" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A5" s="29">
         <v>3</v>
       </c>
@@ -3392,8 +3541,11 @@
       <c r="DX5" s="25" t="s">
         <v>145</v>
       </c>
+      <c r="DY5" s="25" t="s">
+        <v>273</v>
+      </c>
     </row>
-    <row r="6" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A6" s="29">
         <v>4</v>
       </c>
@@ -3850,11 +4002,14 @@
         <f t="shared" si="74"/>
         <v>Excellent</v>
       </c>
-      <c r="DX6" s="39" t="s">
-        <v>247</v>
+      <c r="DX6" s="33" t="s">
+        <v>246</v>
+      </c>
+      <c r="DY6" s="25" t="s">
+        <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A7" s="29">
         <v>5</v>
       </c>
@@ -4312,10 +4467,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX7" s="26" t="s">
-        <v>248</v>
+        <v>247</v>
+      </c>
+      <c r="DY7" s="25" t="s">
+        <v>275</v>
       </c>
     </row>
-    <row r="8" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A8" s="29">
         <v>6</v>
       </c>
@@ -4775,8 +4933,11 @@
       <c r="DX8" s="25" t="s">
         <v>147</v>
       </c>
+      <c r="DY8" s="25" t="s">
+        <v>276</v>
+      </c>
     </row>
-    <row r="9" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A9" s="29">
         <v>7</v>
       </c>
@@ -5236,8 +5397,11 @@
       <c r="DX9" s="25" t="s">
         <v>146</v>
       </c>
+      <c r="DY9" s="25" t="s">
+        <v>277</v>
+      </c>
     </row>
-    <row r="10" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A10" s="29">
         <v>8</v>
       </c>
@@ -5694,11 +5858,14 @@
         <f t="shared" si="74"/>
         <v>Excellent</v>
       </c>
-      <c r="DX10" s="40" t="s">
-        <v>249</v>
+      <c r="DX10" s="34" t="s">
+        <v>248</v>
+      </c>
+      <c r="DY10" s="25" t="s">
+        <v>278</v>
       </c>
     </row>
-    <row r="11" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A11" s="29">
         <v>9</v>
       </c>
@@ -6155,11 +6322,14 @@
         <f t="shared" si="74"/>
         <v>Excellent</v>
       </c>
-      <c r="DX11" s="40" t="s">
-        <v>250</v>
+      <c r="DX11" s="34" t="s">
+        <v>249</v>
+      </c>
+      <c r="DY11" s="25" t="s">
+        <v>279</v>
       </c>
     </row>
-    <row r="12" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A12" s="29">
         <v>10</v>
       </c>
@@ -6619,8 +6789,11 @@
       <c r="DX12" s="25" t="s">
         <v>155</v>
       </c>
+      <c r="DY12" s="25" t="s">
+        <v>280</v>
+      </c>
     </row>
-    <row r="13" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A13" s="29">
         <v>11</v>
       </c>
@@ -7078,10 +7251,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX13" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
+      </c>
+      <c r="DY13" s="25" t="s">
+        <v>281</v>
       </c>
     </row>
-    <row r="14" spans="1:128" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:129" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="29">
         <v>12</v>
       </c>
@@ -7541,8 +7717,11 @@
       <c r="DX14" s="25" t="s">
         <v>148</v>
       </c>
+      <c r="DY14" s="25" t="s">
+        <v>282</v>
+      </c>
     </row>
-    <row r="15" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A15" s="29">
         <v>13</v>
       </c>
@@ -8002,8 +8181,11 @@
       <c r="DX15" s="25" t="s">
         <v>156</v>
       </c>
+      <c r="DY15" s="25" t="s">
+        <v>283</v>
+      </c>
     </row>
-    <row r="16" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A16" s="29">
         <v>14</v>
       </c>
@@ -8017,7 +8199,7 @@
         <v>106</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>141</v>
@@ -8463,8 +8645,11 @@
       <c r="DX16" s="25" t="s">
         <v>149</v>
       </c>
+      <c r="DY16" s="25" t="s">
+        <v>284</v>
+      </c>
     </row>
-    <row r="17" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A17" s="29">
         <v>15</v>
       </c>
@@ -8922,10 +9107,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX17" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
+      </c>
+      <c r="DY17" s="25" t="s">
+        <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A18" s="29">
         <v>16</v>
       </c>
@@ -9385,8 +9573,11 @@
       <c r="DX18" s="26" t="s">
         <v>157</v>
       </c>
+      <c r="DY18" s="25" t="s">
+        <v>286</v>
+      </c>
     </row>
-    <row r="19" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A19" s="29">
         <v>17</v>
       </c>
@@ -9846,8 +10037,11 @@
       <c r="DX19" s="25" t="s">
         <v>150</v>
       </c>
+      <c r="DY19" s="25" t="s">
+        <v>287</v>
+      </c>
     </row>
-    <row r="20" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A20" s="29">
         <v>18</v>
       </c>
@@ -9858,10 +10052,10 @@
         <v>182412018</v>
       </c>
       <c r="D20" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>141</v>
@@ -10307,8 +10501,11 @@
       <c r="DX20" s="25" t="s">
         <v>151</v>
       </c>
+      <c r="DY20" s="25" t="s">
+        <v>288</v>
+      </c>
     </row>
-    <row r="21" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <v>19</v>
       </c>
@@ -10768,13 +10965,16 @@
       <c r="DX21" s="25" t="s">
         <v>158</v>
       </c>
+      <c r="DY21" s="25" t="s">
+        <v>289</v>
+      </c>
     </row>
-    <row r="22" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A22" s="29">
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C22" s="15">
         <v>182412020</v>
@@ -11227,10 +11427,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX22" s="25" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="DY22" s="25" t="s">
+        <v>290</v>
       </c>
     </row>
-    <row r="23" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A23" s="29">
         <v>21</v>
       </c>
@@ -11241,10 +11444,10 @@
         <v>182412021</v>
       </c>
       <c r="D23" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>235</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>236</v>
       </c>
       <c r="F23" s="7" t="s">
         <v>230</v>
@@ -11690,8 +11893,11 @@
       <c r="DX23" s="25" t="s">
         <v>159</v>
       </c>
+      <c r="DY23" s="25" t="s">
+        <v>291</v>
+      </c>
     </row>
-    <row r="24" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A24" s="29">
         <v>22</v>
       </c>
@@ -12149,10 +12355,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX24" s="25" t="s">
-        <v>262</v>
+        <v>261</v>
+      </c>
+      <c r="DY24" s="25" t="s">
+        <v>292</v>
       </c>
     </row>
-    <row r="25" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A25" s="29">
         <v>23</v>
       </c>
@@ -12612,8 +12821,11 @@
       <c r="DX25" s="25" t="s">
         <v>152</v>
       </c>
+      <c r="DY25" s="25" t="s">
+        <v>293</v>
+      </c>
     </row>
-    <row r="26" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A26" s="29">
         <v>24</v>
       </c>
@@ -13073,8 +13285,11 @@
       <c r="DX26" s="25" t="s">
         <v>160</v>
       </c>
+      <c r="DY26" s="25" t="s">
+        <v>294</v>
+      </c>
     </row>
-    <row r="27" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A27" s="29">
         <v>25</v>
       </c>
@@ -13088,13 +13303,13 @@
         <v>106</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>230</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H27" s="5">
         <v>75.75</v>
@@ -13532,8 +13747,9 @@
         <v>Excellent</v>
       </c>
       <c r="DX27" s="25"/>
+      <c r="DY27" s="25"/>
     </row>
-    <row r="28" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
         <v>26</v>
       </c>
@@ -13553,7 +13769,7 @@
         <v>141</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H28" s="5">
         <v>75.75</v>
@@ -13991,10 +14207,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX28" s="25" t="s">
-        <v>263</v>
+        <v>262</v>
+      </c>
+      <c r="DY28" s="25" t="s">
+        <v>295</v>
       </c>
     </row>
-    <row r="29" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A29" s="29">
         <v>27</v>
       </c>
@@ -14005,10 +14224,10 @@
         <v>182412030</v>
       </c>
       <c r="D29" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="E29" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>141</v>
@@ -14454,8 +14673,11 @@
       <c r="DX29" s="25" t="s">
         <v>153</v>
       </c>
+      <c r="DY29" s="25" t="s">
+        <v>296</v>
+      </c>
     </row>
-    <row r="30" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A30" s="29">
         <v>28</v>
       </c>
@@ -14913,10 +15135,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX30" s="25" t="s">
-        <v>252</v>
+        <v>251</v>
+      </c>
+      <c r="DY30" s="25" t="s">
+        <v>297</v>
       </c>
     </row>
-    <row r="31" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A31" s="29">
         <v>29</v>
       </c>
@@ -15373,11 +15598,14 @@
         <f t="shared" si="74"/>
         <v>Excellent</v>
       </c>
-      <c r="DX31" s="40" t="s">
-        <v>264</v>
+      <c r="DX31" s="34" t="s">
+        <v>263</v>
+      </c>
+      <c r="DY31" s="25" t="s">
+        <v>298</v>
       </c>
     </row>
-    <row r="32" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A32" s="29">
         <v>30</v>
       </c>
@@ -15835,10 +16063,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX32" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
+      </c>
+      <c r="DY32" s="25" t="s">
+        <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A33" s="29">
         <v>31</v>
       </c>
@@ -16296,10 +16527,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX33" s="25" t="s">
-        <v>265</v>
+        <v>264</v>
+      </c>
+      <c r="DY33" s="25" t="s">
+        <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A34" s="29">
         <v>32</v>
       </c>
@@ -16757,10 +16991,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX34" s="25" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="DY34" s="25" t="s">
+        <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A35" s="29">
         <v>33</v>
       </c>
@@ -17220,8 +17457,11 @@
       <c r="DX35" s="25" t="s">
         <v>161</v>
       </c>
+      <c r="DY35" s="25" t="s">
+        <v>302</v>
+      </c>
     </row>
-    <row r="36" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A36" s="29">
         <v>34</v>
       </c>
@@ -17681,8 +17921,11 @@
       <c r="DX36" s="25" t="s">
         <v>162</v>
       </c>
+      <c r="DY36" s="25" t="s">
+        <v>303</v>
+      </c>
     </row>
-    <row r="37" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A37" s="29">
         <v>35</v>
       </c>
@@ -18142,8 +18385,11 @@
       <c r="DX37" s="25" t="s">
         <v>163</v>
       </c>
+      <c r="DY37" s="25" t="s">
+        <v>304</v>
+      </c>
     </row>
-    <row r="38" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A38" s="29">
         <v>36</v>
       </c>
@@ -18603,8 +18849,11 @@
       <c r="DX38" s="25" t="s">
         <v>154</v>
       </c>
+      <c r="DY38" s="25" t="s">
+        <v>305</v>
+      </c>
     </row>
-    <row r="39" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A39" s="29">
         <v>37</v>
       </c>
@@ -19064,8 +19313,11 @@
       <c r="DX39" s="25" t="s">
         <v>164</v>
       </c>
+      <c r="DY39" s="25" t="s">
+        <v>306</v>
+      </c>
     </row>
-    <row r="40" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A40" s="29">
         <v>38</v>
       </c>
@@ -19525,8 +19777,11 @@
       <c r="DX40" s="25" t="s">
         <v>165</v>
       </c>
+      <c r="DY40" s="25" t="s">
+        <v>307</v>
+      </c>
     </row>
-    <row r="41" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A41" s="29">
         <v>39</v>
       </c>
@@ -19984,10 +20239,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX41" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="DY41" s="25" t="s">
+        <v>308</v>
       </c>
     </row>
-    <row r="42" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A42" s="29">
         <v>40</v>
       </c>
@@ -20004,7 +20262,7 @@
         <v>181</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G42" s="28" t="s">
         <v>221</v>
@@ -20446,10 +20704,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX42" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
+      </c>
+      <c r="DY42" s="25" t="s">
+        <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A43" s="29">
         <v>41</v>
       </c>
@@ -20469,7 +20730,7 @@
         <v>141</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H43" s="5">
         <v>78.75</v>
@@ -20907,10 +21168,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX43" s="25" t="s">
-        <v>257</v>
+        <v>256</v>
+      </c>
+      <c r="DY43" s="25" t="s">
+        <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A44" s="29">
         <v>42</v>
       </c>
@@ -21368,10 +21632,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX44" s="25" t="s">
-        <v>268</v>
+        <v>267</v>
+      </c>
+      <c r="DY44" s="25" t="s">
+        <v>311</v>
       </c>
     </row>
-    <row r="45" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A45" s="29">
         <v>43</v>
       </c>
@@ -21382,7 +21649,7 @@
         <v>182412048</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>180</v>
@@ -21830,10 +22097,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX45" s="25" t="s">
-        <v>237</v>
+        <v>236</v>
+      </c>
+      <c r="DY45" s="25" t="s">
+        <v>312</v>
       </c>
     </row>
-    <row r="46" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A46" s="29">
         <v>44</v>
       </c>
@@ -22291,10 +22561,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX46" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
+      </c>
+      <c r="DY46" s="25" t="s">
+        <v>313</v>
       </c>
     </row>
-    <row r="47" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A47" s="29">
         <v>45</v>
       </c>
@@ -22754,8 +23027,11 @@
       <c r="DX47" s="25" t="s">
         <v>166</v>
       </c>
+      <c r="DY47" s="25" t="s">
+        <v>314</v>
+      </c>
     </row>
-    <row r="48" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A48" s="29">
         <v>46</v>
       </c>
@@ -23213,8 +23489,9 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX48" s="25"/>
+      <c r="DY48" s="25"/>
     </row>
-    <row r="49" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A49" s="29">
         <v>47</v>
       </c>
@@ -23672,10 +23949,13 @@
         <v>Excellent</v>
       </c>
       <c r="DX49" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
+      </c>
+      <c r="DY49" s="25" t="s">
+        <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:128" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:129" x14ac:dyDescent="0.25">
       <c r="A50" s="29">
         <v>48</v>
       </c>
@@ -24132,26 +24412,29 @@
         <f t="shared" si="74"/>
         <v>Excellent</v>
       </c>
-      <c r="DX50" s="40" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="53" spans="1:128" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
-        <v>232</v>
+      <c r="DX50" s="34" t="s">
+        <v>265</v>
+      </c>
+      <c r="DY50" s="25" t="s">
+        <v>316</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="38">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
+  <mergeCells count="39">
+    <mergeCell ref="DY1:DY2"/>
+    <mergeCell ref="DX1:DX2"/>
+    <mergeCell ref="CT1:CX1"/>
+    <mergeCell ref="CY1:DC1"/>
+    <mergeCell ref="DD1:DH1"/>
+    <mergeCell ref="DI1:DM1"/>
+    <mergeCell ref="DT1:DT2"/>
+    <mergeCell ref="DS1:DS2"/>
+    <mergeCell ref="DR1:DR2"/>
+    <mergeCell ref="CE1:CI1"/>
+    <mergeCell ref="CJ1:CN1"/>
+    <mergeCell ref="DU1:DU2"/>
+    <mergeCell ref="DV1:DV2"/>
+    <mergeCell ref="DW1:DW2"/>
     <mergeCell ref="R1:V1"/>
     <mergeCell ref="CO1:CS1"/>
     <mergeCell ref="BA1:BE1"/>
@@ -24168,19 +24451,15 @@
     <mergeCell ref="BP1:BT1"/>
     <mergeCell ref="BU1:BY1"/>
     <mergeCell ref="BZ1:CD1"/>
-    <mergeCell ref="CE1:CI1"/>
-    <mergeCell ref="CJ1:CN1"/>
-    <mergeCell ref="DU1:DU2"/>
-    <mergeCell ref="DV1:DV2"/>
-    <mergeCell ref="DW1:DW2"/>
-    <mergeCell ref="DX1:DX2"/>
-    <mergeCell ref="CT1:CX1"/>
-    <mergeCell ref="CY1:DC1"/>
-    <mergeCell ref="DD1:DH1"/>
-    <mergeCell ref="DI1:DM1"/>
-    <mergeCell ref="DT1:DT2"/>
-    <mergeCell ref="DS1:DS2"/>
-    <mergeCell ref="DR1:DR2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
perubahan data dan penambahan R.meta
</commit_message>
<xml_diff>
--- a/S1 Keperawatan/RPL/RPL 3/Transkip Nilai RPL3.xlsx
+++ b/S1 Keperawatan/RPL/RPL 3/Transkip Nilai RPL3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\S1 Keperawatan\RPL\RPL 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3092F6C-8A8B-4C82-B8C7-77894CA22E37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12E2BFC7-5C94-47D9-8950-E397759DB505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F6728395-340D-414D-8D40-C463D1B813FA}"/>
+    <workbookView xWindow="-21697" yWindow="-2460" windowWidth="21795" windowHeight="12975" xr2:uid="{F6728395-340D-414D-8D40-C463D1B813FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Transkip" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="318">
   <si>
     <t>NO</t>
   </si>
@@ -588,141 +588,6 @@
     <t>28 Oktober 1991</t>
   </si>
   <si>
-    <t>996 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>997 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>998 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>999 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1000 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1001 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1002 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1003 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1004 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1005 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1006 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1007 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1008 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1009 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1010 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1011 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1012 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1013 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1014 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1015 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1016 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1017 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1018 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1020 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1023 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1024 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1025 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1026 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1027 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1028 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1029 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1030 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1031 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1032 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1033 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1034 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1035 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1036 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1038 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1039 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1040 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1041 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1042 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1043 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1044 / 11 / VIII / 2025</t>
-  </si>
-  <si>
     <t>Abang Suhermantri</t>
   </si>
   <si>
@@ -735,9 +600,6 @@
     <t xml:space="preserve">Namu Sira Sira </t>
   </si>
   <si>
-    <t>7 November</t>
-  </si>
-  <si>
     <t xml:space="preserve">Pinang Sori </t>
   </si>
   <si>
@@ -747,15 +609,6 @@
     <t>Hubungan Kehadiran Orang Tua dengan Kecemasan Anak Saat Pemberian Obat Intravena Line di Ruang Rawat Inap Anak RSUD Natuna</t>
   </si>
   <si>
-    <t>1021 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1022 / 11 / VIII / 2025</t>
-  </si>
-  <si>
-    <t>1037 / 11 / VIII / 2025</t>
-  </si>
-  <si>
     <t>Batam</t>
   </si>
   <si>
@@ -985,6 +838,156 @@
   </si>
   <si>
     <t>The Relationship between Anxiety and Hypertension Compliance in Elderly Women in the Sedanau Primary Health Care Center UPTD Working Area</t>
+  </si>
+  <si>
+    <t>996 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>997 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>998 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>999 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1000 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1001 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1002 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1004 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1005 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1006 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1007 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1009 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1010 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1011 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1012 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1013 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1014 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1015 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1017 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1018 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1019 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1021 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1022 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1023 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1024 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1025 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1026 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1027 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1028 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1029 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1030 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1031 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1032 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1033 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1034 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1036 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1038 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1039 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1040 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1041 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1043 / 11 / X / 2025</t>
+  </si>
+  <si>
+    <t>1003 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>1008 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>1016 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>1020 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>1035 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>1037 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>1042 / 11 / XI / 2025</t>
+  </si>
+  <si>
+    <t>Faktor Faktor Yang Berhubungan Dengan Kualitas hidup Pasien Pasca Stroke Di Poliklinik Neurologi RSUD Natuna</t>
+  </si>
+  <si>
+    <t>Factors Associated with the Quality of Life of Post-Stroke Patients at the Neurology Polyclinic of Natuna Regional Hospital</t>
   </si>
 </sst>
 </file>
@@ -1547,10 +1550,10 @@
   <dimension ref="A1:DY50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="CI3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="DD29" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="DA21" sqref="DA21"/>
+      <selection pane="bottomRight" activeCell="DL41" sqref="DL41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1791,7 +1794,7 @@
         <v>144</v>
       </c>
       <c r="DY1" s="41" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
     </row>
     <row r="2" spans="1:129" x14ac:dyDescent="0.25">
@@ -2158,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="C3" s="15">
         <v>182412001</v>
@@ -2173,7 +2176,7 @@
         <v>141</v>
       </c>
       <c r="G3" s="28" t="s">
-        <v>184</v>
+        <v>268</v>
       </c>
       <c r="H3" s="5">
         <v>75.75</v>
@@ -2611,10 +2614,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX3" s="25" t="s">
-        <v>258</v>
+        <v>209</v>
       </c>
       <c r="DY3" s="25" t="s">
-        <v>271</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:129" x14ac:dyDescent="0.2">
@@ -2637,7 +2640,7 @@
         <v>141</v>
       </c>
       <c r="G4" s="28" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
       <c r="H4" s="5">
         <v>77.25</v>
@@ -3075,10 +3078,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX4" s="25" t="s">
-        <v>259</v>
+        <v>210</v>
       </c>
       <c r="DY4" s="25" t="s">
-        <v>272</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:129" x14ac:dyDescent="0.2">
@@ -3101,7 +3104,7 @@
         <v>141</v>
       </c>
       <c r="G5" s="28" t="s">
-        <v>186</v>
+        <v>270</v>
       </c>
       <c r="H5" s="5">
         <v>80.25</v>
@@ -3542,7 +3545,7 @@
         <v>145</v>
       </c>
       <c r="DY5" s="25" t="s">
-        <v>273</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:129" x14ac:dyDescent="0.2">
@@ -3565,7 +3568,7 @@
         <v>141</v>
       </c>
       <c r="G6" s="28" t="s">
-        <v>187</v>
+        <v>271</v>
       </c>
       <c r="H6" s="5">
         <v>71</v>
@@ -4003,10 +4006,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX6" s="33" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="DY6" s="25" t="s">
-        <v>274</v>
+        <v>225</v>
       </c>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.2">
@@ -4029,7 +4032,7 @@
         <v>141</v>
       </c>
       <c r="G7" s="28" t="s">
-        <v>188</v>
+        <v>272</v>
       </c>
       <c r="H7" s="5">
         <v>75.75</v>
@@ -4467,10 +4470,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX7" s="26" t="s">
-        <v>247</v>
+        <v>198</v>
       </c>
       <c r="DY7" s="25" t="s">
-        <v>275</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:129" x14ac:dyDescent="0.2">
@@ -4493,7 +4496,7 @@
         <v>141</v>
       </c>
       <c r="G8" s="28" t="s">
-        <v>189</v>
+        <v>273</v>
       </c>
       <c r="H8" s="5">
         <v>77.25</v>
@@ -4934,7 +4937,7 @@
         <v>147</v>
       </c>
       <c r="DY8" s="25" t="s">
-        <v>276</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:129" x14ac:dyDescent="0.2">
@@ -4957,7 +4960,7 @@
         <v>141</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>190</v>
+        <v>274</v>
       </c>
       <c r="H9" s="5">
         <v>82</v>
@@ -5398,7 +5401,7 @@
         <v>146</v>
       </c>
       <c r="DY9" s="25" t="s">
-        <v>277</v>
+        <v>228</v>
       </c>
     </row>
     <row r="10" spans="1:129" x14ac:dyDescent="0.25">
@@ -5418,10 +5421,10 @@
         <v>182</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>191</v>
+        <v>309</v>
       </c>
       <c r="H10" s="5">
         <v>82</v>
@@ -5859,10 +5862,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX10" s="34" t="s">
-        <v>248</v>
+        <v>199</v>
       </c>
       <c r="DY10" s="25" t="s">
-        <v>278</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:129" x14ac:dyDescent="0.25">
@@ -5885,7 +5888,7 @@
         <v>141</v>
       </c>
       <c r="G11" s="28" t="s">
-        <v>192</v>
+        <v>275</v>
       </c>
       <c r="H11" s="5">
         <v>74</v>
@@ -6323,10 +6326,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX11" s="34" t="s">
-        <v>249</v>
+        <v>200</v>
       </c>
       <c r="DY11" s="25" t="s">
-        <v>279</v>
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:129" x14ac:dyDescent="0.2">
@@ -6349,7 +6352,7 @@
         <v>141</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>193</v>
+        <v>276</v>
       </c>
       <c r="H12" s="5">
         <v>72.5</v>
@@ -6790,7 +6793,7 @@
         <v>155</v>
       </c>
       <c r="DY12" s="25" t="s">
-        <v>280</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.2">
@@ -6813,7 +6816,7 @@
         <v>141</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>194</v>
+        <v>277</v>
       </c>
       <c r="H13" s="5">
         <v>77.25</v>
@@ -7251,10 +7254,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX13" s="25" t="s">
-        <v>260</v>
+        <v>211</v>
       </c>
       <c r="DY13" s="25" t="s">
-        <v>281</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:129" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -7277,7 +7280,7 @@
         <v>141</v>
       </c>
       <c r="G14" s="28" t="s">
-        <v>195</v>
+        <v>278</v>
       </c>
       <c r="H14" s="5">
         <v>83.5</v>
@@ -7718,7 +7721,7 @@
         <v>148</v>
       </c>
       <c r="DY14" s="25" t="s">
-        <v>282</v>
+        <v>233</v>
       </c>
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.2">
@@ -7738,10 +7741,10 @@
         <v>171</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="G15" s="28" t="s">
-        <v>196</v>
+        <v>310</v>
       </c>
       <c r="H15" s="5">
         <v>71</v>
@@ -8182,7 +8185,7 @@
         <v>156</v>
       </c>
       <c r="DY15" s="25" t="s">
-        <v>283</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:129" x14ac:dyDescent="0.2">
@@ -8199,13 +8202,13 @@
         <v>106</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>242</v>
+        <v>193</v>
       </c>
       <c r="F16" s="7" t="s">
         <v>141</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>197</v>
+        <v>279</v>
       </c>
       <c r="H16" s="5">
         <v>77.25</v>
@@ -8646,7 +8649,7 @@
         <v>149</v>
       </c>
       <c r="DY16" s="25" t="s">
-        <v>284</v>
+        <v>235</v>
       </c>
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.2">
@@ -8669,7 +8672,7 @@
         <v>141</v>
       </c>
       <c r="G17" s="28" t="s">
-        <v>198</v>
+        <v>280</v>
       </c>
       <c r="H17" s="5">
         <v>80.25</v>
@@ -9107,10 +9110,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX17" s="25" t="s">
-        <v>268</v>
+        <v>219</v>
       </c>
       <c r="DY17" s="25" t="s">
-        <v>285</v>
+        <v>236</v>
       </c>
     </row>
     <row r="18" spans="1:129" x14ac:dyDescent="0.2">
@@ -9133,7 +9136,7 @@
         <v>141</v>
       </c>
       <c r="G18" s="28" t="s">
-        <v>199</v>
+        <v>281</v>
       </c>
       <c r="H18" s="5">
         <v>78.75</v>
@@ -9574,7 +9577,7 @@
         <v>157</v>
       </c>
       <c r="DY18" s="25" t="s">
-        <v>286</v>
+        <v>237</v>
       </c>
     </row>
     <row r="19" spans="1:129" x14ac:dyDescent="0.2">
@@ -9597,7 +9600,7 @@
         <v>141</v>
       </c>
       <c r="G19" s="28" t="s">
-        <v>200</v>
+        <v>282</v>
       </c>
       <c r="H19" s="5">
         <v>78.75</v>
@@ -10038,7 +10041,7 @@
         <v>150</v>
       </c>
       <c r="DY19" s="25" t="s">
-        <v>287</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="1:129" x14ac:dyDescent="0.2">
@@ -10052,16 +10055,16 @@
         <v>182412018</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>243</v>
+        <v>194</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>244</v>
+        <v>195</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>141</v>
       </c>
       <c r="G20" s="28" t="s">
-        <v>201</v>
+        <v>283</v>
       </c>
       <c r="H20" s="5">
         <v>77.25</v>
@@ -10502,7 +10505,7 @@
         <v>151</v>
       </c>
       <c r="DY20" s="25" t="s">
-        <v>288</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="1:129" x14ac:dyDescent="0.2">
@@ -10525,7 +10528,7 @@
         <v>141</v>
       </c>
       <c r="G21" s="28" t="s">
-        <v>202</v>
+        <v>284</v>
       </c>
       <c r="H21" s="5">
         <v>72.5</v>
@@ -10966,7 +10969,7 @@
         <v>158</v>
       </c>
       <c r="DY21" s="25" t="s">
-        <v>289</v>
+        <v>240</v>
       </c>
     </row>
     <row r="22" spans="1:129" x14ac:dyDescent="0.2">
@@ -10974,7 +10977,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>269</v>
+        <v>220</v>
       </c>
       <c r="C22" s="15">
         <v>182412020</v>
@@ -10989,7 +10992,7 @@
         <v>141</v>
       </c>
       <c r="G22" s="28" t="s">
-        <v>203</v>
+        <v>285</v>
       </c>
       <c r="H22" s="5">
         <v>75.75</v>
@@ -11427,10 +11430,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX22" s="25" t="s">
-        <v>250</v>
+        <v>201</v>
       </c>
       <c r="DY22" s="25" t="s">
-        <v>290</v>
+        <v>241</v>
       </c>
     </row>
     <row r="23" spans="1:129" x14ac:dyDescent="0.2">
@@ -11444,16 +11447,16 @@
         <v>182412021</v>
       </c>
       <c r="D23" s="15" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>235</v>
+        <v>189</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="G23" s="28" t="s">
-        <v>204</v>
+        <v>311</v>
       </c>
       <c r="H23" s="5">
         <v>75.75</v>
@@ -11848,7 +11851,7 @@
         <v>4</v>
       </c>
       <c r="DM23" s="2">
-        <f t="shared" si="66"/>
+        <f>DK23*DL23</f>
         <v>14</v>
       </c>
       <c r="DN23" s="23">
@@ -11894,7 +11897,7 @@
         <v>159</v>
       </c>
       <c r="DY23" s="25" t="s">
-        <v>291</v>
+        <v>242</v>
       </c>
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.2">
@@ -11917,7 +11920,7 @@
         <v>141</v>
       </c>
       <c r="G24" s="28" t="s">
-        <v>205</v>
+        <v>286</v>
       </c>
       <c r="H24" s="5">
         <v>71</v>
@@ -12355,10 +12358,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX24" s="25" t="s">
-        <v>261</v>
+        <v>212</v>
       </c>
       <c r="DY24" s="25" t="s">
-        <v>292</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.2">
@@ -12381,7 +12384,7 @@
         <v>141</v>
       </c>
       <c r="G25" s="28" t="s">
-        <v>206</v>
+        <v>287</v>
       </c>
       <c r="H25" s="5">
         <v>75.75</v>
@@ -12822,7 +12825,7 @@
         <v>152</v>
       </c>
       <c r="DY25" s="25" t="s">
-        <v>293</v>
+        <v>244</v>
       </c>
     </row>
     <row r="26" spans="1:129" x14ac:dyDescent="0.2">
@@ -12845,7 +12848,7 @@
         <v>141</v>
       </c>
       <c r="G26" s="28" t="s">
-        <v>207</v>
+        <v>288</v>
       </c>
       <c r="H26" s="5">
         <v>74</v>
@@ -13286,7 +13289,7 @@
         <v>160</v>
       </c>
       <c r="DY26" s="25" t="s">
-        <v>294</v>
+        <v>245</v>
       </c>
     </row>
     <row r="27" spans="1:129" x14ac:dyDescent="0.2">
@@ -13303,13 +13306,13 @@
         <v>106</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>245</v>
+        <v>196</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="G27" s="28" t="s">
-        <v>237</v>
+        <v>312</v>
       </c>
       <c r="H27" s="5">
         <v>75.75</v>
@@ -13746,8 +13749,12 @@
         <f t="shared" si="74"/>
         <v>Excellent</v>
       </c>
-      <c r="DX27" s="25"/>
-      <c r="DY27" s="25"/>
+      <c r="DX27" s="25" t="s">
+        <v>316</v>
+      </c>
+      <c r="DY27" s="25" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="28" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A28" s="29">
@@ -13769,7 +13776,7 @@
         <v>141</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>238</v>
+        <v>289</v>
       </c>
       <c r="H28" s="5">
         <v>75.75</v>
@@ -14207,10 +14214,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX28" s="25" t="s">
-        <v>262</v>
+        <v>213</v>
       </c>
       <c r="DY28" s="25" t="s">
-        <v>295</v>
+        <v>246</v>
       </c>
     </row>
     <row r="29" spans="1:129" x14ac:dyDescent="0.2">
@@ -14224,16 +14231,16 @@
         <v>182412030</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>240</v>
+        <v>191</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>241</v>
+        <v>192</v>
       </c>
       <c r="F29" s="7" t="s">
         <v>141</v>
       </c>
       <c r="G29" s="28" t="s">
-        <v>208</v>
+        <v>290</v>
       </c>
       <c r="H29" s="5">
         <v>78.75</v>
@@ -14674,7 +14681,7 @@
         <v>153</v>
       </c>
       <c r="DY29" s="25" t="s">
-        <v>296</v>
+        <v>247</v>
       </c>
     </row>
     <row r="30" spans="1:129" x14ac:dyDescent="0.2">
@@ -14697,7 +14704,7 @@
         <v>141</v>
       </c>
       <c r="G30" s="28" t="s">
-        <v>209</v>
+        <v>291</v>
       </c>
       <c r="H30" s="5">
         <v>74</v>
@@ -15135,10 +15142,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX30" s="25" t="s">
-        <v>251</v>
+        <v>202</v>
       </c>
       <c r="DY30" s="25" t="s">
-        <v>297</v>
+        <v>248</v>
       </c>
     </row>
     <row r="31" spans="1:129" x14ac:dyDescent="0.25">
@@ -15161,7 +15168,7 @@
         <v>141</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>210</v>
+        <v>292</v>
       </c>
       <c r="H31" s="5">
         <v>74</v>
@@ -15599,10 +15606,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX31" s="34" t="s">
-        <v>263</v>
+        <v>214</v>
       </c>
       <c r="DY31" s="25" t="s">
-        <v>298</v>
+        <v>249</v>
       </c>
     </row>
     <row r="32" spans="1:129" x14ac:dyDescent="0.2">
@@ -15625,7 +15632,7 @@
         <v>141</v>
       </c>
       <c r="G32" s="28" t="s">
-        <v>211</v>
+        <v>293</v>
       </c>
       <c r="H32" s="5">
         <v>78.75</v>
@@ -16063,10 +16070,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX32" s="25" t="s">
-        <v>252</v>
+        <v>203</v>
       </c>
       <c r="DY32" s="25" t="s">
-        <v>299</v>
+        <v>250</v>
       </c>
     </row>
     <row r="33" spans="1:129" x14ac:dyDescent="0.2">
@@ -16089,7 +16096,7 @@
         <v>141</v>
       </c>
       <c r="G33" s="28" t="s">
-        <v>212</v>
+        <v>294</v>
       </c>
       <c r="H33" s="5">
         <v>72.5</v>
@@ -16527,10 +16534,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX33" s="25" t="s">
-        <v>264</v>
+        <v>215</v>
       </c>
       <c r="DY33" s="25" t="s">
-        <v>300</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="1:129" x14ac:dyDescent="0.2">
@@ -16553,7 +16560,7 @@
         <v>141</v>
       </c>
       <c r="G34" s="28" t="s">
-        <v>213</v>
+        <v>295</v>
       </c>
       <c r="H34" s="5">
         <v>77.25</v>
@@ -16991,10 +16998,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX34" s="25" t="s">
-        <v>253</v>
+        <v>204</v>
       </c>
       <c r="DY34" s="25" t="s">
-        <v>301</v>
+        <v>252</v>
       </c>
     </row>
     <row r="35" spans="1:129" x14ac:dyDescent="0.2">
@@ -17017,7 +17024,7 @@
         <v>141</v>
       </c>
       <c r="G35" s="28" t="s">
-        <v>214</v>
+        <v>296</v>
       </c>
       <c r="H35" s="5">
         <v>75.75</v>
@@ -17458,7 +17465,7 @@
         <v>161</v>
       </c>
       <c r="DY35" s="25" t="s">
-        <v>302</v>
+        <v>253</v>
       </c>
     </row>
     <row r="36" spans="1:129" x14ac:dyDescent="0.2">
@@ -17481,7 +17488,7 @@
         <v>141</v>
       </c>
       <c r="G36" s="28" t="s">
-        <v>215</v>
+        <v>297</v>
       </c>
       <c r="H36" s="5">
         <v>78.75</v>
@@ -17922,7 +17929,7 @@
         <v>162</v>
       </c>
       <c r="DY36" s="25" t="s">
-        <v>303</v>
+        <v>254</v>
       </c>
     </row>
     <row r="37" spans="1:129" x14ac:dyDescent="0.2">
@@ -17945,7 +17952,7 @@
         <v>141</v>
       </c>
       <c r="G37" s="28" t="s">
-        <v>216</v>
+        <v>298</v>
       </c>
       <c r="H37" s="5">
         <v>77.25</v>
@@ -18386,7 +18393,7 @@
         <v>163</v>
       </c>
       <c r="DY37" s="25" t="s">
-        <v>304</v>
+        <v>255</v>
       </c>
     </row>
     <row r="38" spans="1:129" x14ac:dyDescent="0.2">
@@ -18409,7 +18416,7 @@
         <v>141</v>
       </c>
       <c r="G38" s="28" t="s">
-        <v>217</v>
+        <v>299</v>
       </c>
       <c r="H38" s="5">
         <v>80.25</v>
@@ -18850,7 +18857,7 @@
         <v>154</v>
       </c>
       <c r="DY38" s="25" t="s">
-        <v>305</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:129" x14ac:dyDescent="0.2">
@@ -18873,7 +18880,7 @@
         <v>141</v>
       </c>
       <c r="G39" s="28" t="s">
-        <v>218</v>
+        <v>300</v>
       </c>
       <c r="H39" s="5">
         <v>77.25</v>
@@ -19314,7 +19321,7 @@
         <v>164</v>
       </c>
       <c r="DY39" s="25" t="s">
-        <v>306</v>
+        <v>257</v>
       </c>
     </row>
     <row r="40" spans="1:129" x14ac:dyDescent="0.2">
@@ -19337,7 +19344,7 @@
         <v>141</v>
       </c>
       <c r="G40" s="28" t="s">
-        <v>219</v>
+        <v>301</v>
       </c>
       <c r="H40" s="5">
         <v>80.25</v>
@@ -19778,7 +19785,7 @@
         <v>165</v>
       </c>
       <c r="DY40" s="25" t="s">
-        <v>307</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:129" x14ac:dyDescent="0.2">
@@ -19801,7 +19808,7 @@
         <v>141</v>
       </c>
       <c r="G41" s="28" t="s">
-        <v>220</v>
+        <v>302</v>
       </c>
       <c r="H41" s="5">
         <v>80.25</v>
@@ -20239,10 +20246,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX41" s="25" t="s">
-        <v>254</v>
+        <v>205</v>
       </c>
       <c r="DY41" s="25" t="s">
-        <v>308</v>
+        <v>259</v>
       </c>
     </row>
     <row r="42" spans="1:129" x14ac:dyDescent="0.2">
@@ -20262,10 +20269,10 @@
         <v>181</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>233</v>
+        <v>185</v>
       </c>
       <c r="G42" s="28" t="s">
-        <v>221</v>
+        <v>313</v>
       </c>
       <c r="H42" s="5">
         <v>71</v>
@@ -20704,10 +20711,10 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="DX42" s="25" t="s">
-        <v>255</v>
+        <v>206</v>
       </c>
       <c r="DY42" s="25" t="s">
-        <v>309</v>
+        <v>260</v>
       </c>
     </row>
     <row r="43" spans="1:129" x14ac:dyDescent="0.2">
@@ -20730,7 +20737,7 @@
         <v>141</v>
       </c>
       <c r="G43" s="28" t="s">
-        <v>239</v>
+        <v>303</v>
       </c>
       <c r="H43" s="5">
         <v>78.75</v>
@@ -21168,10 +21175,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX43" s="25" t="s">
-        <v>256</v>
+        <v>207</v>
       </c>
       <c r="DY43" s="25" t="s">
-        <v>310</v>
+        <v>261</v>
       </c>
     </row>
     <row r="44" spans="1:129" x14ac:dyDescent="0.2">
@@ -21191,10 +21198,10 @@
         <v>172</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="G44" s="28" t="s">
-        <v>222</v>
+        <v>314</v>
       </c>
       <c r="H44" s="5">
         <v>78.75</v>
@@ -21632,10 +21639,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX44" s="25" t="s">
-        <v>267</v>
+        <v>218</v>
       </c>
       <c r="DY44" s="25" t="s">
-        <v>311</v>
+        <v>262</v>
       </c>
     </row>
     <row r="45" spans="1:129" x14ac:dyDescent="0.2">
@@ -21649,7 +21656,7 @@
         <v>182412048</v>
       </c>
       <c r="D45" s="10" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>180</v>
@@ -21658,7 +21665,7 @@
         <v>141</v>
       </c>
       <c r="G45" s="28" t="s">
-        <v>223</v>
+        <v>304</v>
       </c>
       <c r="H45" s="5">
         <v>75.75</v>
@@ -22097,10 +22104,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX45" s="25" t="s">
-        <v>236</v>
+        <v>190</v>
       </c>
       <c r="DY45" s="25" t="s">
-        <v>312</v>
+        <v>263</v>
       </c>
     </row>
     <row r="46" spans="1:129" x14ac:dyDescent="0.2">
@@ -22123,7 +22130,7 @@
         <v>141</v>
       </c>
       <c r="G46" s="28" t="s">
-        <v>224</v>
+        <v>305</v>
       </c>
       <c r="H46" s="5">
         <v>83.5</v>
@@ -22561,10 +22568,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX46" s="25" t="s">
-        <v>266</v>
+        <v>217</v>
       </c>
       <c r="DY46" s="25" t="s">
-        <v>313</v>
+        <v>264</v>
       </c>
     </row>
     <row r="47" spans="1:129" x14ac:dyDescent="0.2">
@@ -22587,7 +22594,7 @@
         <v>141</v>
       </c>
       <c r="G47" s="28" t="s">
-        <v>225</v>
+        <v>306</v>
       </c>
       <c r="H47" s="5">
         <v>80.25</v>
@@ -23028,7 +23035,7 @@
         <v>166</v>
       </c>
       <c r="DY47" s="25" t="s">
-        <v>314</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:129" x14ac:dyDescent="0.2">
@@ -23051,7 +23058,7 @@
         <v>141</v>
       </c>
       <c r="G48" s="28" t="s">
-        <v>226</v>
+        <v>307</v>
       </c>
       <c r="H48" s="5">
         <v>74</v>
@@ -23508,10 +23515,10 @@
         <v>178</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="G49" s="28" t="s">
-        <v>227</v>
+        <v>315</v>
       </c>
       <c r="H49" s="5">
         <v>71</v>
@@ -23949,10 +23956,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX49" s="25" t="s">
-        <v>257</v>
+        <v>208</v>
       </c>
       <c r="DY49" s="25" t="s">
-        <v>315</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:129" x14ac:dyDescent="0.25">
@@ -23975,7 +23982,7 @@
         <v>141</v>
       </c>
       <c r="G50" s="28" t="s">
-        <v>228</v>
+        <v>308</v>
       </c>
       <c r="H50" s="5">
         <v>78.75</v>
@@ -24413,10 +24420,10 @@
         <v>Excellent</v>
       </c>
       <c r="DX50" s="34" t="s">
-        <v>265</v>
+        <v>216</v>
       </c>
       <c r="DY50" s="25" t="s">
-        <v>316</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>